<commit_message>
Global PAPA and Irminger MOAS Cal and CSV
Reviewed Cal and ingest sheets for Global PAPA and Irminger.  Corrected
reference designators where applicable.  Created ingest CSV's where
needed including global profiling gliders.
</commit_message>
<xml_diff>
--- a/GI05MOAS-PG528/Omaha_Cal_Info_GI05MOAS-PG528_00001.xlsx
+++ b/GI05MOAS-PG528/Omaha_Cal_Info_GI05MOAS-PG528_00001.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\Ingest sheets\ingestion-csvs\GI05MOAS-PG528\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12260" yWindow="2480" windowWidth="25320" windowHeight="10600" tabRatio="377"/>
+    <workbookView xWindow="12255" yWindow="2475" windowWidth="25320" windowHeight="10605" tabRatio="377" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -30,7 +35,7 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$98</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$402</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -88,27 +93,6 @@
   </si>
   <si>
     <t>No calibration coefficient</t>
-  </si>
-  <si>
-    <t>GI05MOAS-PG003-01-CTDGVM000</t>
-  </si>
-  <si>
-    <t>GI05MOAS-PG003-02-DOSTAM000</t>
-  </si>
-  <si>
-    <t>GI05MOAS-PG003-03-NUTNRM000</t>
-  </si>
-  <si>
-    <t>GI05MOAS-PG003-04-PARADM000</t>
-  </si>
-  <si>
-    <t>GI05MOAS-PG003-05-FLORTM000</t>
-  </si>
-  <si>
-    <t>GI05MOAS-PG003-06-FLORTO000</t>
-  </si>
-  <si>
-    <t>GI05MOAS-PG003-00-ENG000000</t>
   </si>
   <si>
     <t>CC_dark_counts_volume_scatter</t>
@@ -209,6 +193,27 @@
       </rPr>
       <t>528</t>
     </r>
+  </si>
+  <si>
+    <t>GI05MOAS-PG528-01-CTDGVM000</t>
+  </si>
+  <si>
+    <t>GI05MOAS-PG528-02-DOSTAM000</t>
+  </si>
+  <si>
+    <t>GI05MOAS-PG528-06-FLORTO000</t>
+  </si>
+  <si>
+    <t>GI05MOAS-PG528-00-ENG000000</t>
+  </si>
+  <si>
+    <t>GI05MOAS-PG528-05-NUTNRM000</t>
+  </si>
+  <si>
+    <t>GI05MOAS-PG528-06-PARADM000</t>
+  </si>
+  <si>
+    <t>GI05MOAS-PG528-03-FLORTM000</t>
   </si>
 </sst>
 </file>
@@ -710,6 +715,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1004,20 +1012,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="20.83203125" customWidth="1"/>
-    <col min="9" max="10" width="15.83203125" customWidth="1"/>
-    <col min="11" max="11" width="29.1640625" customWidth="1"/>
-    <col min="12" max="12" width="17.83203125" customWidth="1"/>
-    <col min="13" max="13" width="18.33203125" customWidth="1"/>
+    <col min="1" max="8" width="20.85546875" customWidth="1"/>
+    <col min="9" max="10" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="29.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30">
+    <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1052,9 +1060,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="6" customFormat="1" ht="15">
+    <row r="2" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B2" s="8">
         <v>528</v>
@@ -1070,16 +1078,16 @@
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="36" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="H2" s="36" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="I2" s="43">
         <v>200</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="22">
@@ -1104,24 +1112,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.5" customWidth="1"/>
-    <col min="6" max="6" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15">
+    <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1141,9 +1149,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1">
+    <row r="2" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B2" s="21">
         <v>528</v>
@@ -1165,7 +1173,7 @@
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:12" s="4" customFormat="1">
+    <row r="3" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -1179,9 +1187,9 @@
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:12" s="4" customFormat="1">
+    <row r="4" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B4" s="21">
         <v>528</v>
@@ -1203,7 +1211,7 @@
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:12" s="4" customFormat="1">
+    <row r="5" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
       <c r="B5" s="21"/>
       <c r="C5" s="14"/>
@@ -1217,9 +1225,9 @@
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
     </row>
-    <row r="6" spans="1:12" s="4" customFormat="1">
+    <row r="6" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="B6" s="21">
         <v>528</v>
@@ -1236,7 +1244,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="4" customFormat="1">
+    <row r="7" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="21"/>
       <c r="C7" s="14"/>
@@ -1250,9 +1258,9 @@
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:12" s="4" customFormat="1">
+    <row r="8" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B8" s="21">
         <v>528</v>
@@ -1269,7 +1277,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="4" customFormat="1">
+    <row r="9" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="21"/>
       <c r="C9" s="14"/>
@@ -1283,9 +1291,9 @@
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:12" s="4" customFormat="1">
+    <row r="10" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="34" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B10" s="21">
         <v>528</v>
@@ -1297,13 +1305,13 @@
         <v>3777</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F10" s="30">
         <v>44</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="H10" s="24"/>
       <c r="I10" s="12"/>
@@ -1311,9 +1319,9 @@
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="1:12" s="4" customFormat="1">
+    <row r="11" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="37" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B11" s="38">
         <v>528</v>
@@ -1325,7 +1333,7 @@
         <v>3777</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F11" s="31">
         <v>1.5829999999999999E-6</v>
@@ -1337,9 +1345,9 @@
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
     </row>
-    <row r="12" spans="1:12" s="4" customFormat="1">
+    <row r="12" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="37" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B12" s="38">
         <v>528</v>
@@ -1351,7 +1359,7 @@
         <v>3777</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F12" s="30">
         <v>45</v>
@@ -1363,9 +1371,9 @@
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" s="4" customFormat="1">
+    <row r="13" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="37" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B13" s="38">
         <v>528</v>
@@ -1377,7 +1385,7 @@
         <v>3777</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F13" s="30">
         <v>7.3000000000000001E-3</v>
@@ -1389,9 +1397,9 @@
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:12" s="4" customFormat="1">
+    <row r="14" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="37" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B14" s="38">
         <v>528</v>
@@ -1403,7 +1411,7 @@
         <v>3777</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F14" s="30">
         <v>43</v>
@@ -1415,9 +1423,9 @@
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:12" s="4" customFormat="1">
+    <row r="15" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="37" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B15" s="38">
         <v>528</v>
@@ -1429,7 +1437,7 @@
         <v>3777</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F15" s="30">
         <v>9.0700000000000003E-2</v>
@@ -1441,9 +1449,9 @@
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:12" s="4" customFormat="1">
+    <row r="16" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="37" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B16" s="38">
         <v>528</v>
@@ -1455,7 +1463,7 @@
         <v>3777</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F16" s="41">
         <v>124</v>
@@ -1467,9 +1475,9 @@
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
     </row>
-    <row r="17" spans="1:12" s="4" customFormat="1">
+    <row r="17" spans="1:16" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="37" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B17" s="38">
         <v>528</v>
@@ -1481,7 +1489,7 @@
         <v>3777</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F17" s="28">
         <v>700</v>
@@ -1493,9 +1501,9 @@
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
     </row>
-    <row r="18" spans="1:12" s="4" customFormat="1">
+    <row r="18" spans="1:16" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="37" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B18" s="38">
         <v>528</v>
@@ -1507,7 +1515,7 @@
         <v>3777</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F18" s="42">
         <v>1.0760000000000001</v>
@@ -1519,9 +1527,9 @@
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
     </row>
-    <row r="19" spans="1:12" s="4" customFormat="1">
+    <row r="19" spans="1:16" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="37" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B19" s="38">
         <v>528</v>
@@ -1533,7 +1541,7 @@
         <v>3777</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F19" s="29">
         <v>3.9E-2</v>
@@ -1545,7 +1553,7 @@
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
     </row>
-    <row r="20" spans="1:12" s="4" customFormat="1">
+    <row r="20" spans="1:16" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
       <c r="B20" s="21"/>
       <c r="C20" s="14"/>
@@ -1559,285 +1567,276 @@
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
     </row>
-    <row r="21" spans="1:12" s="4" customFormat="1">
-      <c r="A21" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="21">
-        <v>528</v>
-      </c>
-      <c r="C21" s="14">
-        <v>1</v>
-      </c>
-      <c r="D21" s="14">
+    <row r="21" spans="1:16" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H21" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="I21" s="21">
+        <v>528</v>
+      </c>
+      <c r="J21" s="14">
+        <v>1</v>
+      </c>
+      <c r="K21" s="14">
         <v>1240</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="L21" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="M21" s="32">
+        <v>650</v>
+      </c>
+      <c r="N21" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="O21" s="25"/>
+    </row>
+    <row r="22" spans="1:16" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H22" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="38">
+        <v>528</v>
+      </c>
+      <c r="J22" s="39">
+        <v>1</v>
+      </c>
+      <c r="K22" s="39">
+        <v>1240</v>
+      </c>
+      <c r="L22" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="M22" s="32">
+        <v>41</v>
+      </c>
+      <c r="N22" s="24"/>
+      <c r="O22" s="25"/>
+    </row>
+    <row r="23" spans="1:16" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H23" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23" s="38">
+        <v>528</v>
+      </c>
+      <c r="J23" s="39">
+        <v>1</v>
+      </c>
+      <c r="K23" s="39">
+        <v>1240</v>
+      </c>
+      <c r="L23" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="M23" s="33">
+        <v>3.602E-6</v>
+      </c>
+      <c r="N23" s="24"/>
+      <c r="O23" s="25"/>
+    </row>
+    <row r="24" spans="1:16" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H24" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" s="38">
+        <v>528</v>
+      </c>
+      <c r="J24" s="39">
+        <v>1</v>
+      </c>
+      <c r="K24" s="39">
+        <v>1240</v>
+      </c>
+      <c r="L24" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="M24" s="32">
+        <v>532</v>
+      </c>
+      <c r="N24" s="24"/>
+      <c r="O24" s="25"/>
+    </row>
+    <row r="25" spans="1:16" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H25" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25" s="38">
+        <v>528</v>
+      </c>
+      <c r="J25" s="39">
+        <v>1</v>
+      </c>
+      <c r="K25" s="39">
+        <v>1240</v>
+      </c>
+      <c r="L25" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="32">
-        <v>650</v>
-      </c>
-      <c r="G21" s="24" t="s">
+      <c r="M25" s="32">
+        <v>39</v>
+      </c>
+      <c r="N25" s="24"/>
+      <c r="O25" s="25"/>
+    </row>
+    <row r="26" spans="1:16" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H26" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="H21" s="25"/>
-    </row>
-    <row r="22" spans="1:12" s="4" customFormat="1">
-      <c r="A22" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="38">
-        <v>528</v>
-      </c>
-      <c r="C22" s="39">
-        <v>1</v>
-      </c>
-      <c r="D22" s="39">
+      <c r="I26" s="38">
+        <v>528</v>
+      </c>
+      <c r="J26" s="39">
+        <v>1</v>
+      </c>
+      <c r="K26" s="39">
         <v>1240</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="L26" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="32">
-        <v>41</v>
-      </c>
-      <c r="G22" s="24"/>
-      <c r="H22" s="25"/>
-    </row>
-    <row r="23" spans="1:12" s="4" customFormat="1">
-      <c r="A23" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="38">
-        <v>528</v>
-      </c>
-      <c r="C23" s="39">
-        <v>1</v>
-      </c>
-      <c r="D23" s="39">
+      <c r="M26" s="33">
+        <v>7.1539999999999996E-6</v>
+      </c>
+      <c r="N26" s="24"/>
+      <c r="O26" s="25"/>
+    </row>
+    <row r="27" spans="1:16" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H27" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="I27" s="38">
+        <v>528</v>
+      </c>
+      <c r="J27" s="39">
+        <v>1</v>
+      </c>
+      <c r="K27" s="39">
         <v>1240</v>
       </c>
-      <c r="E23" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="33">
-        <v>3.602E-6</v>
-      </c>
-      <c r="G23" s="24"/>
-      <c r="H23" s="25"/>
-    </row>
-    <row r="24" spans="1:12" s="4" customFormat="1">
-      <c r="A24" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="38">
-        <v>528</v>
-      </c>
-      <c r="C24" s="39">
-        <v>1</v>
-      </c>
-      <c r="D24" s="39">
+      <c r="L27" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="M27" s="32">
+        <v>470</v>
+      </c>
+      <c r="N27" s="24"/>
+      <c r="O27" s="25"/>
+    </row>
+    <row r="28" spans="1:16" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H28" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="I28" s="38">
+        <v>528</v>
+      </c>
+      <c r="J28" s="39">
+        <v>1</v>
+      </c>
+      <c r="K28" s="39">
         <v>1240</v>
       </c>
-      <c r="E24" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24" s="32">
-        <v>532</v>
-      </c>
-      <c r="G24" s="24"/>
-      <c r="H24" s="25"/>
-    </row>
-    <row r="25" spans="1:12" s="4" customFormat="1">
-      <c r="A25" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="38">
-        <v>528</v>
-      </c>
-      <c r="C25" s="39">
-        <v>1</v>
-      </c>
-      <c r="D25" s="39">
+      <c r="L28" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="M28" s="32">
+        <v>50</v>
+      </c>
+      <c r="N28" s="24"/>
+      <c r="O28" s="25"/>
+    </row>
+    <row r="29" spans="1:16" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H29" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="I29" s="38">
+        <v>528</v>
+      </c>
+      <c r="J29" s="39">
+        <v>1</v>
+      </c>
+      <c r="K29" s="39">
         <v>1240</v>
       </c>
-      <c r="E25" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" s="32">
-        <v>39</v>
-      </c>
-      <c r="G25" s="24"/>
-      <c r="H25" s="25"/>
-    </row>
-    <row r="26" spans="1:12" s="4" customFormat="1">
-      <c r="A26" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="38">
-        <v>528</v>
-      </c>
-      <c r="C26" s="39">
-        <v>1</v>
-      </c>
-      <c r="D26" s="39">
+      <c r="L29" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="M29" s="33">
+        <v>1.1029999999999999E-5</v>
+      </c>
+      <c r="N29" s="24"/>
+      <c r="O29" s="25"/>
+    </row>
+    <row r="30" spans="1:16" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H30" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="I30" s="38">
+        <v>528</v>
+      </c>
+      <c r="J30" s="39">
+        <v>1</v>
+      </c>
+      <c r="K30" s="39">
         <v>1240</v>
       </c>
-      <c r="E26" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="F26" s="33">
-        <v>7.1539999999999996E-6</v>
-      </c>
-      <c r="G26" s="24"/>
-      <c r="H26" s="25"/>
-    </row>
-    <row r="27" spans="1:12" s="4" customFormat="1">
-      <c r="A27" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="38">
-        <v>528</v>
-      </c>
-      <c r="C27" s="39">
-        <v>1</v>
-      </c>
-      <c r="D27" s="39">
+      <c r="L30" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="M30" s="41">
+        <v>124</v>
+      </c>
+      <c r="N30" s="35"/>
+      <c r="O30" s="35"/>
+      <c r="P30" s="12"/>
+    </row>
+    <row r="31" spans="1:16" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H31" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="I31" s="38">
+        <v>528</v>
+      </c>
+      <c r="J31" s="39">
+        <v>1</v>
+      </c>
+      <c r="K31" s="39">
         <v>1240</v>
       </c>
-      <c r="E27" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" s="32">
-        <v>470</v>
-      </c>
-      <c r="G27" s="24"/>
-      <c r="H27" s="25"/>
-    </row>
-    <row r="28" spans="1:12" s="4" customFormat="1">
-      <c r="A28" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="38">
-        <v>528</v>
-      </c>
-      <c r="C28" s="39">
-        <v>1</v>
-      </c>
-      <c r="D28" s="39">
+      <c r="L31" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="M31" s="42">
+        <v>1.0760000000000001</v>
+      </c>
+      <c r="N31" s="35"/>
+      <c r="O31" s="35"/>
+      <c r="P31" s="12"/>
+    </row>
+    <row r="32" spans="1:16" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H32" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="I32" s="38">
+        <v>528</v>
+      </c>
+      <c r="J32" s="39">
+        <v>1</v>
+      </c>
+      <c r="K32" s="39">
         <v>1240</v>
       </c>
-      <c r="E28" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="F28" s="32">
-        <v>50</v>
-      </c>
-      <c r="G28" s="24"/>
-      <c r="H28" s="25"/>
-    </row>
-    <row r="29" spans="1:12" s="4" customFormat="1">
-      <c r="A29" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="38">
-        <v>528</v>
-      </c>
-      <c r="C29" s="39">
-        <v>1</v>
-      </c>
-      <c r="D29" s="39">
-        <v>1240</v>
-      </c>
-      <c r="E29" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="F29" s="33">
-        <v>1.1029999999999999E-5</v>
-      </c>
-      <c r="G29" s="24"/>
-      <c r="H29" s="25"/>
-    </row>
-    <row r="30" spans="1:12" s="4" customFormat="1">
-      <c r="A30" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="38">
-        <v>528</v>
-      </c>
-      <c r="C30" s="39">
-        <v>1</v>
-      </c>
-      <c r="D30" s="39">
-        <v>1240</v>
-      </c>
-      <c r="E30" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="41">
-        <v>124</v>
-      </c>
-      <c r="G30" s="35"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="12"/>
-    </row>
-    <row r="31" spans="1:12" s="4" customFormat="1">
-      <c r="A31" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" s="38">
-        <v>528</v>
-      </c>
-      <c r="C31" s="39">
-        <v>1</v>
-      </c>
-      <c r="D31" s="39">
-        <v>1240</v>
-      </c>
-      <c r="E31" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="F31" s="42">
-        <v>1.0760000000000001</v>
-      </c>
-      <c r="G31" s="35"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
-    </row>
-    <row r="32" spans="1:12" s="4" customFormat="1">
-      <c r="A32" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" s="38">
-        <v>528</v>
-      </c>
-      <c r="C32" s="39">
-        <v>1</v>
-      </c>
-      <c r="D32" s="39">
-        <v>1240</v>
-      </c>
-      <c r="E32" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="F32" s="29">
+      <c r="L32" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="M32" s="29">
         <v>3.9E-2</v>
       </c>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
-    </row>
-    <row r="33" spans="1:12" s="4" customFormat="1">
+      <c r="N32" s="35"/>
+      <c r="O32" s="35"/>
+      <c r="P32" s="12"/>
+    </row>
+    <row r="33" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
       <c r="B33" s="21"/>
       <c r="C33" s="14"/>
@@ -1851,9 +1850,9 @@
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
     </row>
-    <row r="34" spans="1:12" s="4" customFormat="1">
+    <row r="34" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="B34" s="21">
         <v>528</v>
@@ -1875,7 +1874,7 @@
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
     </row>
-    <row r="35" spans="1:12" s="4" customFormat="1">
+    <row r="35" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>

</xml_diff>